<commit_message>
Small fixes on the flow numbering and figures
</commit_message>
<xml_diff>
--- a/template/aiphoria_template.xlsx
+++ b/template/aiphoria_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABCD0AF-97C6-4E79-BF1E-640F847C84E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9929A2DA-7509-408D-8B1B-382C71D6FFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -108,26 +108,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={A1233539-2DE7-4EBD-8A76-0466F733D277}</author>
-  </authors>
-  <commentList>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{A1233539-2DE7-4EBD-8A76-0466F733D277}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Conversion to ODMT not carbon!</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="130">
   <si>
     <t>Years</t>
   </si>
@@ -364,42 +346,12 @@
     <t>2 columns needed for each indicator (value and comment)</t>
   </si>
   <si>
-    <t>Source_process</t>
-  </si>
-  <si>
-    <t>Transformation_Stage</t>
-  </si>
-  <si>
-    <t>Source_process_location</t>
-  </si>
-  <si>
-    <t>Target_process</t>
-  </si>
-  <si>
-    <t>Target_process_location</t>
-  </si>
-  <si>
-    <t>Source _ID</t>
-  </si>
-  <si>
-    <t>Target_ID</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Data_source_comment</t>
   </si>
   <si>
     <t xml:space="preserve">Conversion_factor_used </t>
   </si>
   <si>
-    <t>Carbon_content_factor</t>
-  </si>
-  <si>
     <t>Carbon_content_source</t>
   </si>
   <si>
@@ -425,9 +377,6 @@
   </si>
   <si>
     <t>Furniture</t>
-  </si>
-  <si>
-    <t>https://excalidraw.com/#json=XTpmhzuJw-3ozVbASdSZz,QuLhsga6HJSHN0nM7kMAMA</t>
   </si>
   <si>
     <t>Residues</t>
@@ -599,6 +548,69 @@
   </si>
   <si>
     <t>Mm3 SWE</t>
+  </si>
+  <si>
+    <t>Source_process*</t>
+  </si>
+  <si>
+    <t>Source_process_location*</t>
+  </si>
+  <si>
+    <t>Target_process*</t>
+  </si>
+  <si>
+    <t>Target_process_location*</t>
+  </si>
+  <si>
+    <t>Source _ID*</t>
+  </si>
+  <si>
+    <t>Target_ID*</t>
+  </si>
+  <si>
+    <t>Value*</t>
+  </si>
+  <si>
+    <t>Unit*</t>
+  </si>
+  <si>
+    <t>Year*</t>
+  </si>
+  <si>
+    <t>Carbon_content_conversion</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://excalidraw.com/#json=acMq06Ek074LvgJQcBgt-,_z-k-OWtxYKdxCtl_tJVQg </t>
   </si>
 </sst>
 </file>
@@ -864,22 +876,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>970055</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>3176</xdr:rowOff>
+      <xdr:colOff>779319</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>64064</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1770902</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>103171</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>311610</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>16634</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Graphic 3">
+        <xdr:cNvPr id="2" name="Graphic 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{186AA4F2-8439-0B6B-4F97-D26DA395FC6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{060A53AB-2C39-4786-AA4D-FFB36F5549BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -901,8 +913,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5194673" y="4676029"/>
-          <a:ext cx="7759700" cy="2606938"/>
+          <a:off x="5004955" y="4618746"/>
+          <a:ext cx="9594155" cy="2723479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1223,14 +1235,6 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="P3" dT="2024-07-05T06:41:30.02" personId="{10F4E90A-0171-4D8D-A06D-5391EEA853D3}" id="{A1233539-2DE7-4EBD-8A76-0466F733D277}">
-    <text>Conversion to ODMT not carbon!</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
   <dimension ref="A1:E13"/>
@@ -1281,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D3" s="31"/>
     </row>
@@ -1305,7 +1309,7 @@
         <v>54</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D5" s="34"/>
     </row>
@@ -1317,7 +1321,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D6" s="30"/>
     </row>
@@ -1383,25 +1387,25 @@
     </row>
     <row r="12" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D13" s="30"/>
     </row>
@@ -1430,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1440,6 +1444,7 @@
     <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" customWidth="1"/>
     <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.453125" customWidth="1"/>
     <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1"/>
@@ -1583,10 +1588,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(B4,":",C4)</f>
@@ -1599,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1612,7 +1617,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
@@ -1620,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D12" si="0">_xlfn.CONCAT(B5,":",C5)</f>
@@ -1636,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1649,7 +1654,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -1657,23 +1662,23 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Residues:FI</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1685,7 +1690,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="R6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -1693,10 +1698,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7" si="1">_xlfn.CONCAT(B7,":",C7)</f>
@@ -1709,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1721,7 +1726,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1729,23 +1734,23 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1757,7 +1762,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1765,23 +1770,23 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Furniture:FI</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1793,7 +1798,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -1801,7 +1806,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -1817,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1829,7 +1834,7 @@
         <v>0.81899999999999995</v>
       </c>
       <c r="R10" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -1837,7 +1842,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1853,7 +1858,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1865,7 +1870,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -1873,23 +1878,23 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Incineration:FI</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1901,7 +1906,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1913,11 +1918,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2034,89 +2039,89 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="25" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="M3" s="25" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="26" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="R3" s="27" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="S3" s="28" t="s">
         <v>22</v>
       </c>
       <c r="T3" s="27" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="U3" s="28" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C4" t="str">
         <f>+_xlfn.XLOOKUP(H4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Source</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F4" t="str">
         <f>+_xlfn.XLOOKUP(I4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" ref="H4:H23" si="0">_xlfn.CONCAT(B4,":",D4)</f>
@@ -2130,45 +2135,45 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L4">
         <v>2021</v>
       </c>
       <c r="N4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P4">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
+      <c r="A5" t="s">
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C5" t="str">
         <f>+_xlfn.XLOOKUP(H5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F5" t="str">
         <f>+_xlfn.XLOOKUP(I5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2182,45 +2187,45 @@
         <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L5">
         <v>2021</v>
       </c>
       <c r="N5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P5">
         <f>0.4238*'Carbon fraction (will be moved)'!C2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q5" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>3</v>
+      <c r="A6" t="s">
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C6" t="str">
         <f>+_xlfn.XLOOKUP(H6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F6" t="str">
         <f>+_xlfn.XLOOKUP(I6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>by_prod</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2234,45 +2239,45 @@
         <v>19.5</v>
       </c>
       <c r="K6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L6">
         <v>2021</v>
       </c>
       <c r="N6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P6">
         <f>0.395*'Carbon fraction (will be moved)'!C2</f>
         <v>0.18959999999999999</v>
       </c>
       <c r="Q6" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>4</v>
+      <c r="A7" t="s">
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C7" t="str">
         <f>+_xlfn.XLOOKUP(H7,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F7" t="str">
         <f>+_xlfn.XLOOKUP(I7,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2292,39 +2297,39 @@
         <v>2021</v>
       </c>
       <c r="N7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P7">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
       <c r="Q7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>5</v>
+      <c r="A8" t="s">
+        <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C8" t="str">
         <f>+_xlfn.XLOOKUP(H8,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F8" t="str">
         <f>+_xlfn.XLOOKUP(I8,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H8" s="4" t="str">
         <f>_xlfn.CONCAT(B8,":",D8)</f>
@@ -2344,39 +2349,39 @@
         <v>2021</v>
       </c>
       <c r="N8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P8">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
+      <c r="A9" t="s">
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C9" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F9" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2396,39 +2401,39 @@
         <v>2021</v>
       </c>
       <c r="N9" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P9">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
       <c r="Q9" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>7</v>
+      <c r="A10" t="s">
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C10" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F10" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2448,38 +2453,38 @@
         <v>2021</v>
       </c>
       <c r="N10" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P10">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>8</v>
+      <c r="A11" t="s">
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F11" t="str">
         <f>+_xlfn.XLOOKUP(I11,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2499,32 +2504,32 @@
         <v>2021</v>
       </c>
       <c r="N11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P11">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q11" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>9</v>
+      <c r="A12" t="s">
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C12" t="str">
         <f>+_xlfn.XLOOKUP(H12,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F12" t="str">
         <f>+_xlfn.XLOOKUP(I12,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
@@ -2545,28 +2550,28 @@
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L12">
         <v>2021</v>
       </c>
       <c r="N12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P12">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q12" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>10</v>
+      <c r="A13" t="s">
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C13" t="str">
         <f>+_xlfn.XLOOKUP(H13,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
@@ -2576,13 +2581,13 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2596,42 +2601,42 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L13">
         <v>2021</v>
       </c>
       <c r="N13" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P13">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q13" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C14" t="str">
         <f>+_xlfn.XLOOKUP(H14,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Source</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F14" t="str">
         <f>+_xlfn.XLOOKUP(I14,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2645,42 +2650,42 @@
         <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L14">
         <v>2022</v>
       </c>
       <c r="N14" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P14">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q14" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C15" t="str">
         <f>+_xlfn.XLOOKUP(H15,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F15" t="str">
         <f>+_xlfn.XLOOKUP(I15,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2694,42 +2699,42 @@
         <v>50</v>
       </c>
       <c r="K15" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L15">
         <v>2022</v>
       </c>
       <c r="N15" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P15">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q15" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C16" t="str">
         <f>+_xlfn.XLOOKUP(H16,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F16" t="str">
         <f>+_xlfn.XLOOKUP(I16,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>by_prod</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2743,42 +2748,42 @@
         <v>19.5</v>
       </c>
       <c r="K16" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L16">
         <v>2022</v>
       </c>
       <c r="N16" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P16">
         <f>0.395*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.18959999999999999</v>
       </c>
       <c r="Q16" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C17" t="str">
         <f>+_xlfn.XLOOKUP(H17,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F17" t="str">
         <f>+_xlfn.XLOOKUP(I17,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2798,36 +2803,36 @@
         <v>2022</v>
       </c>
       <c r="N17" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P17">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
       <c r="Q17" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C18" t="str">
         <f>+_xlfn.XLOOKUP(H18,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F18" t="str">
         <f>+_xlfn.XLOOKUP(I18,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H18" s="4" t="str">
         <f>_xlfn.CONCAT(B18,":",D18)</f>
@@ -2847,36 +2852,36 @@
         <v>2022</v>
       </c>
       <c r="N18" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P18">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q18" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C19" t="str">
         <f>+_xlfn.XLOOKUP(H19,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F19" t="str">
         <f>+_xlfn.XLOOKUP(I19,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2896,36 +2901,36 @@
         <v>2022</v>
       </c>
       <c r="N19" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P19">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
       <c r="Q19" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C20" t="str">
         <f>+_xlfn.XLOOKUP(H20,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F20" t="str">
         <f>+_xlfn.XLOOKUP(I20,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H20" s="4" t="str">
         <f t="shared" ref="H20" si="2">_xlfn.CONCAT(B20,":",D20)</f>
@@ -2945,35 +2950,35 @@
         <v>2022</v>
       </c>
       <c r="N20" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P20">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q20" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F21" t="str">
         <f>+_xlfn.XLOOKUP(I21,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H21" s="4" t="str">
         <f t="shared" ref="H21" si="4">_xlfn.CONCAT(B21,":",D21)</f>
@@ -2993,29 +2998,29 @@
         <v>2022</v>
       </c>
       <c r="N21" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P21">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q21" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C22" t="str">
         <f>+_xlfn.XLOOKUP(H22,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F22" t="str">
         <f>+_xlfn.XLOOKUP(I22,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
@@ -3036,25 +3041,25 @@
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L22">
         <v>2022</v>
       </c>
       <c r="N22" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P22">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q22" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C23" t="str">
         <f>+_xlfn.XLOOKUP(H23,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
@@ -3064,14 +3069,14 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F23" t="str">
         <f>+_xlfn.XLOOKUP(I23,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3085,20 +3090,20 @@
         <v>10</v>
       </c>
       <c r="K23" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L23">
         <v>2022</v>
       </c>
       <c r="N23" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="P23">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q23" s="29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.35">
@@ -3204,7 +3209,7 @@
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C45" s="9" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
@@ -3502,7 +3507,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <drawing r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -3511,7 +3515,7 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3528,13 +3532,13 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>0.48</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3543,18 +3547,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3563,7 +3555,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -3826,24 +3818,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3851,7 +3838,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3868,4 +3855,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>